<commit_message>
update(demo): Modify description column with the new input parameters
</commit_message>
<xml_diff>
--- a/gearshift/demos/gs_input_demo.xlsx
+++ b/gearshift/demos/gs_input_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\European Comision\WLTP\gearshift_calculation_tool\gearshift\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1230D9B2-44F2-4CE4-B1A5-3D01DF66F01E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F00DDF3-5725-4183-B1C9-40938C2106C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="3" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -4965,13 +4965,13 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4986,8 +4986,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17430750" y="200025"/>
-          <a:ext cx="8382000" cy="17002125"/>
+          <a:off x="15135225" y="200026"/>
+          <a:ext cx="8382000" cy="15430500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5027,7 +5027,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>- case:  </a:t>
+            <a:t>case:  </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
@@ -5055,14 +5055,6 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- </a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
@@ -5080,276 +5072,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="1">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>calc_dsc: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>This</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>is a logical scalar (0 = No | 1 = Yes) , specifying</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>if the calculated downscaling value shall be used instead of the</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>the value given by the input parameter Downscaling Percentage. If the value is 1,</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> the downscaling factor will be calculated following the Paragraph 8.3. of Sub-Annex 1. If the value is 0, the downscaling factor defined in the  f_dsc parameter will be used.</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- Apply Downscaling </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(do_dsc): This</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>is a logical scalar (0 = No | 1 = Yes) , specifying if the trace shall</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>be downscaled. [Ref:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Paragraph 8 of Sub-Annex 1]</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- Apply Speed Cap </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(do_cap):</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> This</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>is a logical scalar (0 = No | 1 = Yes) , specifying if the trace shall be</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>capped to the given CappedSpeed. [Ref: Paragraph 9.1 of Sub-Annex 1]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Apply Distance Compensation </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(do_cmp):</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> ApplyDistanceCompensation is a logical scalar (0 = No | 1 = Yes) , specifying it the trace shall be compensated for distance due to capped speeds. [Ref: Paragraph 9.2.1 of Sub-Annex 1]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
             <a:solidFill>
               <a:schemeClr val="bg1"/>
@@ -5363,7 +5085,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Use Calculated Downscaling Percentage </a:t>
+            <a:t>Maximum velocity </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
@@ -5371,32 +5093,7 @@
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>(calc_dsc): This is a logical scalar, specifying if the calculated downscaling value shall be used instead of the the value given by the input parameter DownscalingPercentage. [Ref: Paragraph 8.2 of Sub-Annex 1]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Downscaling Percentage </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(f_dsc): This is a double scalar, specifying the degree of  downscaling. This value will only be used if the input parameter Use Calculated Downscaling Percentage is false. [Ref: Paragraph 8.2 of Sub-Annex 1]</a:t>
+            <a:t>(v_max): The maximum velocity declared by the manofacturer.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6217,13 +5914,13 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>177801</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6238,8 +5935,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7324725" y="377825"/>
-          <a:ext cx="6731000" cy="288925"/>
+          <a:off x="7324725" y="377826"/>
+          <a:ext cx="6731000" cy="6394450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6996,103 +6693,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Safety Margin</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> (</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>SM):</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>The safety margin is accounting for the difference</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>between the stationary full load condition power curve</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>and the power available during transition conditions.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-ES_tradnl" sz="1200" b="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>SM is set to 10 per cent. [Ref:Paragraph 3.4 of Sub-Annex 2]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0">
             <a:solidFill>
               <a:schemeClr val="bg1"/>
@@ -7134,13 +6734,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>200024</xdr:rowOff>
+      <xdr:rowOff>200023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7155,8 +6755,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3152775" y="600074"/>
-          <a:ext cx="5029200" cy="2066926"/>
+          <a:off x="3152775" y="600073"/>
+          <a:ext cx="5029200" cy="2266951"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7359,6 +6959,13 @@
             </a:rPr>
             <a:t>[Ref: Paragraph 2, point h of Sub-Annex 2]</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES_tradnl" sz="1200" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -9235,7 +8842,7 @@
   </sheetPr>
   <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -11415,8 +11022,8 @@
   </sheetPr>
   <dimension ref="A1:D1156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Update(demo): Updated excel files templates with the new logo.
</commit_message>
<xml_diff>
--- a/gearshift/demos/gs_input_demo.xlsx
+++ b/gearshift/demos/gs_input_demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\European Comision\WLTP\gearshift_calculation_tool\gearshift\demos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\European Comision\WLTP\cloned_repo\gearshift_calculation_tool\gearshift\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FD53F5-2BEF-4A99-B222-0F856B44F43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B3E994-EDCB-433B-9E93-769A76BC576E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5C24A396-E983-DB47-8B10-835CCBF80F80}"/>
   </bookViews>
@@ -4902,11 +4902,11 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -4999,20 +4999,25 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>632732</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>687161</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>142883</xdr:rowOff>
+      <xdr:rowOff>20410</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7772400" cy="736332"/>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>20411</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114810</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E644801C-2C4F-4E78-BC23-2938B7405AF3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CADF2BC-3250-46BC-B82A-69580A8DF63F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5034,8 +5039,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1328057" y="1095383"/>
-          <a:ext cx="7772400" cy="736332"/>
+          <a:off x="687161" y="972910"/>
+          <a:ext cx="9048750" cy="856400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5043,7 +5048,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7934,7 +7939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2725CB3C-4165-43BA-BB90-E06CB0E5A43E}">
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:O50"/>
     </sheetView>
   </sheetViews>
@@ -8185,601 +8190,601 @@
     </row>
     <row r="15" spans="1:15" s="16" customFormat="1" ht="15"/>
     <row r="16" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>1410</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
     </row>
     <row r="17" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
     </row>
     <row r="18" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
     </row>
     <row r="19" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
     </row>
     <row r="20" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
     </row>
     <row r="21" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
     </row>
     <row r="22" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
     </row>
     <row r="23" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
     </row>
     <row r="24" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
     </row>
     <row r="25" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
     </row>
     <row r="26" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
     </row>
     <row r="27" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
     </row>
     <row r="28" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
     </row>
     <row r="29" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="22"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
     </row>
     <row r="30" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
     </row>
     <row r="31" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
     </row>
     <row r="32" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
     </row>
     <row r="33" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
     </row>
     <row r="34" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
     </row>
     <row r="35" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
     </row>
     <row r="36" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="O36" s="22"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
     </row>
     <row r="37" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-      <c r="O37" s="22"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
     </row>
     <row r="38" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
     </row>
     <row r="39" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="22"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
     </row>
     <row r="40" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
     </row>
     <row r="41" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="22"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
     </row>
     <row r="42" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="22"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
     </row>
     <row r="43" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
     </row>
     <row r="44" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
     </row>
     <row r="45" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
     </row>
     <row r="46" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
     </row>
     <row r="47" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="23"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
+      <c r="O47" s="23"/>
     </row>
     <row r="48" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="22"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="23"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="23"/>
     </row>
     <row r="49" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A49" s="22"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="22"/>
-      <c r="O49" s="22"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
     </row>
     <row r="50" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="22"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="22"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="23"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
     </row>
     <row r="51" spans="1:15" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A51" s="21"/>

</xml_diff>